<commit_message>
- Code and classes refactor - Remove unnecessary buttons and functionalities
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -1,26 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SINERGIA\Extractor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\python_projects\pdf2csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A8C06B-9F95-44A8-B032-CC3765F77DBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBECFA90-2D52-4789-AAD8-610EF7BADF47}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet3" sheetId="2" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="4" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="5" r:id="rId4"/>
+    <sheet name="Hoja5" sheetId="6" r:id="rId5"/>
+    <sheet name="Hoja6" sheetId="7" r:id="rId6"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
+  <si>
+    <t>ENTRECALLES</t>
+  </si>
   <si>
     <t>TRACKING ID MERCADO LIBRE</t>
   </si>
@@ -28,9 +37,6 @@
     <t>DOMICILIO</t>
   </si>
   <si>
-    <t>ENTRECALLES</t>
-  </si>
-  <si>
     <t>CODIGO POSTAL</t>
   </si>
   <si>
@@ -52,15 +58,15 @@
     <t>DETALLE DEL ENVIO</t>
   </si>
   <si>
+    <t>Munzón y Catriel</t>
+  </si>
+  <si>
     <t>1234</t>
   </si>
   <si>
     <t>Quirno 2085</t>
   </si>
   <si>
-    <t>Munzón y Catriel</t>
-  </si>
-  <si>
     <t>1661</t>
   </si>
   <si>
@@ -82,15 +88,15 @@
     <t>0-1</t>
   </si>
   <si>
+    <t>Timbre 8</t>
+  </si>
+  <si>
     <t>1235</t>
   </si>
   <si>
     <t>Calle Falsa 123</t>
   </si>
   <si>
-    <t>Timbre 8</t>
-  </si>
-  <si>
     <t>1663</t>
   </si>
   <si>
@@ -101,6 +107,15 @@
   </si>
   <si>
     <t>1198751364</t>
+  </si>
+  <si>
+    <t>jghfj f</t>
+  </si>
+  <si>
+    <t>hjg fgh</t>
+  </si>
+  <si>
+    <t>f hgj fg</t>
   </si>
 </sst>
 </file>
@@ -476,24 +491,113 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="A1" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E950EFD8-163C-4EDA-8E6D-AECC8C0C0F68}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B7EAE96-E6C3-4BB4-A992-BF5563ED566A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E3BFCAE-0C56-4E72-A80E-5DBDFCEE1D85}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE3AEE67-AE80-4437-AB29-A523CAE28318}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C41A49-49F6-430B-A0AA-FF6CCFF0584A}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
@@ -517,15 +621,15 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -549,15 +653,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
         <v>22</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
       </c>
       <c r="D3" t="s">
         <v>23</v>
@@ -584,7 +688,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1:C3 D1:J3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:J3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>